<commit_message>
Bass diffusion for maturities
</commit_message>
<xml_diff>
--- a/Data/technological_maturity_readiness.xlsx
+++ b/Data/technological_maturity_readiness.xlsx
@@ -5,21 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{39DECEEF-037C-4F46-93A5-FB68D0FB36EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5359D8E-B9B2-4222-9EB6-263D32716377}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FD589F-F050-4CBF-9731-4E39708FF62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technological_readiness" sheetId="2" r:id="rId1"/>
     <sheet name="technological_readiness_paths" sheetId="3" r:id="rId2"/>
-    <sheet name="Fuel_groups (cheatsheet)" sheetId="4" r:id="rId3"/>
-    <sheet name="scenarios_maturities_27 (OLD)" sheetId="1" r:id="rId4"/>
+    <sheet name="technological_readiness_temp" sheetId="5" r:id="rId3"/>
+    <sheet name="technological_readiness_bass" sheetId="6" r:id="rId4"/>
+    <sheet name="Fuel_groups (cheatsheet)" sheetId="4" r:id="rId5"/>
+    <sheet name="scenarios_maturities_27 (OLD)" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Fuel_groups (cheatsheet)'!$A$1:$C$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Fuel_groups (cheatsheet)'!$A$1:$C$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="74">
   <si>
     <t>Scenario</t>
   </si>
@@ -220,6 +222,48 @@
   <si>
     <t>Hybrid</t>
   </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>t_0</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Mature</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Mature?</t>
+  </si>
+  <si>
+    <t>Fast: increase p and q by 50%</t>
+  </si>
+  <si>
+    <t>Slow: decrease p and q by 50%</t>
+  </si>
+  <si>
+    <t>What should we make random? P, q, or t_0?</t>
+  </si>
+  <si>
+    <t>Answer: p and q jointly. p affects mostly the beginning (when the technology takes off), while q affects the rest of the process</t>
+  </si>
+  <si>
+    <t>variation</t>
+  </si>
+  <si>
+    <t>Base variation (%)</t>
+  </si>
 </sst>
 </file>
 
@@ -361,7 +405,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,8 +615,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -716,8 +772,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -760,8 +825,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -780,8 +846,21 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="35" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="36" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="39" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -821,6 +900,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1593,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4805C95-1AF1-48B1-A4A3-091952BC3BC4}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2962,6 +3042,2623 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861B896F-D644-4444-9C31-F96BFC1BA11D}">
+  <dimension ref="A1:M52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="5">
+        <v>100</v>
+      </c>
+      <c r="E2" s="5">
+        <v>100</v>
+      </c>
+      <c r="F2" s="5">
+        <v>100</v>
+      </c>
+      <c r="G2" s="5">
+        <v>100</v>
+      </c>
+      <c r="H2" s="5">
+        <v>100</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="M3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="5"/>
+      <c r="M4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14">
+        <v>50</v>
+      </c>
+      <c r="F5" s="14">
+        <v>90</v>
+      </c>
+      <c r="G5" s="14">
+        <v>100</v>
+      </c>
+      <c r="H5" s="14">
+        <v>100</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="14">
+        <v>2020</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="M6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14"/>
+      <c r="M7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <v>10</v>
+      </c>
+      <c r="F8" s="12">
+        <v>40</v>
+      </c>
+      <c r="G8" s="12">
+        <v>100</v>
+      </c>
+      <c r="H8" s="12">
+        <v>100</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="12">
+        <v>2020</v>
+      </c>
+      <c r="K8" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="12">
+        <v>10</v>
+      </c>
+      <c r="F9" s="12">
+        <v>30</v>
+      </c>
+      <c r="G9" s="12">
+        <v>50</v>
+      </c>
+      <c r="H9" s="12">
+        <v>80</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="M9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0</v>
+      </c>
+      <c r="E10" s="13">
+        <v>10</v>
+      </c>
+      <c r="F10" s="13">
+        <v>100</v>
+      </c>
+      <c r="G10" s="13">
+        <v>100</v>
+      </c>
+      <c r="H10" s="13">
+        <v>100</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="M10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="16">
+        <v>5</v>
+      </c>
+      <c r="E11" s="16">
+        <v>10</v>
+      </c>
+      <c r="F11" s="16">
+        <v>12</v>
+      </c>
+      <c r="G11" s="16">
+        <v>15</v>
+      </c>
+      <c r="H11" s="16">
+        <v>20</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J11" s="16">
+        <v>2015</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="L11" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="M11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="16">
+        <v>5</v>
+      </c>
+      <c r="E12" s="16">
+        <v>10</v>
+      </c>
+      <c r="F12" s="16">
+        <v>10</v>
+      </c>
+      <c r="G12" s="16">
+        <v>12</v>
+      </c>
+      <c r="H12" s="16">
+        <v>15</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="M12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="17">
+        <v>5</v>
+      </c>
+      <c r="E13" s="17">
+        <v>10</v>
+      </c>
+      <c r="F13" s="17">
+        <v>15</v>
+      </c>
+      <c r="G13" s="17">
+        <v>20</v>
+      </c>
+      <c r="H13" s="17">
+        <v>20</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="M13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="16">
+        <v>0</v>
+      </c>
+      <c r="E14" s="16">
+        <v>1</v>
+      </c>
+      <c r="F14" s="16">
+        <v>4</v>
+      </c>
+      <c r="G14" s="16">
+        <v>7</v>
+      </c>
+      <c r="H14" s="16">
+        <v>10</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="16">
+        <v>2020</v>
+      </c>
+      <c r="K14" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="M14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0</v>
+      </c>
+      <c r="E15" s="16">
+        <v>1</v>
+      </c>
+      <c r="F15" s="16">
+        <v>2</v>
+      </c>
+      <c r="G15" s="16">
+        <v>3</v>
+      </c>
+      <c r="H15" s="16">
+        <v>4</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="M15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="17">
+        <v>0</v>
+      </c>
+      <c r="E16" s="17">
+        <v>1</v>
+      </c>
+      <c r="F16" s="17">
+        <v>7</v>
+      </c>
+      <c r="G16" s="17">
+        <v>10</v>
+      </c>
+      <c r="H16" s="17">
+        <v>15</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="M16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="5">
+        <v>100</v>
+      </c>
+      <c r="E17" s="5">
+        <v>100</v>
+      </c>
+      <c r="F17" s="5">
+        <v>100</v>
+      </c>
+      <c r="G17" s="5">
+        <v>100</v>
+      </c>
+      <c r="H17" s="5">
+        <v>100</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
+      <c r="K17" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="5">
+        <v>100</v>
+      </c>
+      <c r="E18" s="5">
+        <v>100</v>
+      </c>
+      <c r="F18" s="5">
+        <v>100</v>
+      </c>
+      <c r="G18" s="5">
+        <v>100</v>
+      </c>
+      <c r="H18" s="5">
+        <v>100</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="M18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="6">
+        <v>100</v>
+      </c>
+      <c r="E19" s="6">
+        <v>100</v>
+      </c>
+      <c r="F19" s="6">
+        <v>100</v>
+      </c>
+      <c r="G19" s="6">
+        <v>100</v>
+      </c>
+      <c r="H19" s="6">
+        <v>100</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="M19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="5">
+        <v>100</v>
+      </c>
+      <c r="E20" s="5">
+        <v>100</v>
+      </c>
+      <c r="F20" s="5">
+        <v>100</v>
+      </c>
+      <c r="G20" s="5">
+        <v>100</v>
+      </c>
+      <c r="H20" s="5">
+        <v>100</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J20" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" t="s">
+        <v>64</v>
+      </c>
+      <c r="M20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="5">
+        <v>100</v>
+      </c>
+      <c r="E21" s="5">
+        <v>100</v>
+      </c>
+      <c r="F21" s="5">
+        <v>100</v>
+      </c>
+      <c r="G21" s="5">
+        <v>100</v>
+      </c>
+      <c r="H21" s="5">
+        <v>100</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="M21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="6">
+        <v>100</v>
+      </c>
+      <c r="E22" s="6">
+        <v>100</v>
+      </c>
+      <c r="F22" s="6">
+        <v>100</v>
+      </c>
+      <c r="G22" s="6">
+        <v>100</v>
+      </c>
+      <c r="H22" s="6">
+        <v>100</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="M22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="5">
+        <v>10</v>
+      </c>
+      <c r="E23" s="5">
+        <v>20</v>
+      </c>
+      <c r="F23" s="5">
+        <v>30</v>
+      </c>
+      <c r="G23" s="5">
+        <v>30</v>
+      </c>
+      <c r="H23" s="5">
+        <v>50</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23" s="5">
+        <v>2010</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="L23" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="5">
+        <v>10</v>
+      </c>
+      <c r="E24" s="5">
+        <v>20</v>
+      </c>
+      <c r="F24" s="5">
+        <v>30</v>
+      </c>
+      <c r="G24" s="5">
+        <v>30</v>
+      </c>
+      <c r="H24" s="5">
+        <v>50</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="M24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="6">
+        <v>10</v>
+      </c>
+      <c r="E25" s="6">
+        <v>20</v>
+      </c>
+      <c r="F25" s="6">
+        <v>30</v>
+      </c>
+      <c r="G25" s="6">
+        <v>30</v>
+      </c>
+      <c r="H25" s="6">
+        <v>50</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="M25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>5</v>
+      </c>
+      <c r="G26" s="12">
+        <v>30</v>
+      </c>
+      <c r="H26" s="12">
+        <v>50</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J26" s="12">
+        <v>2025</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="M26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="12">
+        <v>0</v>
+      </c>
+      <c r="E27" s="12">
+        <v>0</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
+      </c>
+      <c r="G27" s="12">
+        <v>20</v>
+      </c>
+      <c r="H27" s="12">
+        <v>40</v>
+      </c>
+      <c r="I27" s="12"/>
+      <c r="M27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0</v>
+      </c>
+      <c r="F28" s="13">
+        <v>25</v>
+      </c>
+      <c r="G28" s="13">
+        <v>50</v>
+      </c>
+      <c r="H28" s="13">
+        <v>60</v>
+      </c>
+      <c r="I28" s="12"/>
+      <c r="M28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0</v>
+      </c>
+      <c r="E29" s="12">
+        <v>0</v>
+      </c>
+      <c r="F29" s="12">
+        <v>5</v>
+      </c>
+      <c r="G29" s="12">
+        <v>30</v>
+      </c>
+      <c r="H29" s="12">
+        <v>60</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J29" s="12">
+        <v>2025</v>
+      </c>
+      <c r="K29" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="L29" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="M29">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="12">
+        <v>0</v>
+      </c>
+      <c r="E30" s="12">
+        <v>0</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0</v>
+      </c>
+      <c r="G30" s="12">
+        <v>10</v>
+      </c>
+      <c r="H30" s="12">
+        <v>30</v>
+      </c>
+      <c r="I30" s="12"/>
+      <c r="M30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="13">
+        <v>0</v>
+      </c>
+      <c r="E31" s="13">
+        <v>0</v>
+      </c>
+      <c r="F31" s="13">
+        <v>15</v>
+      </c>
+      <c r="G31" s="13">
+        <v>45</v>
+      </c>
+      <c r="H31" s="13">
+        <v>80</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="M31">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="16">
+        <v>0</v>
+      </c>
+      <c r="E32" s="16">
+        <v>0</v>
+      </c>
+      <c r="F32" s="16">
+        <v>5</v>
+      </c>
+      <c r="G32" s="16">
+        <v>80</v>
+      </c>
+      <c r="H32" s="16">
+        <v>100</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J32" s="16">
+        <v>2028</v>
+      </c>
+      <c r="K32" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="L32" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="M32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="16">
+        <v>0</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0</v>
+      </c>
+      <c r="F33" s="16">
+        <v>5</v>
+      </c>
+      <c r="G33" s="16">
+        <v>30</v>
+      </c>
+      <c r="H33" s="16">
+        <v>60</v>
+      </c>
+      <c r="I33" s="16"/>
+      <c r="M33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="17">
+        <v>0</v>
+      </c>
+      <c r="E34" s="17">
+        <v>0</v>
+      </c>
+      <c r="F34" s="17">
+        <v>5</v>
+      </c>
+      <c r="G34" s="17">
+        <v>100</v>
+      </c>
+      <c r="H34" s="17">
+        <v>100</v>
+      </c>
+      <c r="I34" s="16"/>
+      <c r="M34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="16">
+        <v>0</v>
+      </c>
+      <c r="E35" s="16">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16">
+        <v>5</v>
+      </c>
+      <c r="G35" s="16">
+        <v>80</v>
+      </c>
+      <c r="H35" s="16">
+        <v>100</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" s="16">
+        <v>2028</v>
+      </c>
+      <c r="K35" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="L35" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="M35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="16">
+        <v>0</v>
+      </c>
+      <c r="E36" s="16">
+        <v>0</v>
+      </c>
+      <c r="F36" s="16">
+        <v>5</v>
+      </c>
+      <c r="G36" s="16">
+        <v>30</v>
+      </c>
+      <c r="H36" s="16">
+        <v>60</v>
+      </c>
+      <c r="I36" s="16"/>
+      <c r="M36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="17">
+        <v>0</v>
+      </c>
+      <c r="E37" s="17">
+        <v>0</v>
+      </c>
+      <c r="F37" s="17">
+        <v>5</v>
+      </c>
+      <c r="G37" s="17">
+        <v>100</v>
+      </c>
+      <c r="H37" s="17">
+        <v>100</v>
+      </c>
+      <c r="I37" s="16"/>
+      <c r="M37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="5">
+        <v>100</v>
+      </c>
+      <c r="E38" s="5">
+        <v>100</v>
+      </c>
+      <c r="F38" s="5">
+        <v>100</v>
+      </c>
+      <c r="G38" s="5">
+        <v>100</v>
+      </c>
+      <c r="H38" s="5">
+        <v>100</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K38" t="s">
+        <v>64</v>
+      </c>
+      <c r="L38" t="s">
+        <v>64</v>
+      </c>
+      <c r="M38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="5">
+        <v>100</v>
+      </c>
+      <c r="E39" s="5">
+        <v>100</v>
+      </c>
+      <c r="F39" s="5">
+        <v>100</v>
+      </c>
+      <c r="G39" s="5">
+        <v>100</v>
+      </c>
+      <c r="H39" s="5">
+        <v>100</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="M39">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" s="6">
+        <v>100</v>
+      </c>
+      <c r="E40" s="6">
+        <v>100</v>
+      </c>
+      <c r="F40" s="6">
+        <v>100</v>
+      </c>
+      <c r="G40" s="6">
+        <v>100</v>
+      </c>
+      <c r="H40" s="6">
+        <v>100</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="M40">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41" s="5">
+        <v>100</v>
+      </c>
+      <c r="E41" s="5">
+        <v>100</v>
+      </c>
+      <c r="F41" s="5">
+        <v>100</v>
+      </c>
+      <c r="G41" s="5">
+        <v>100</v>
+      </c>
+      <c r="H41" s="5">
+        <v>100</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J41" t="s">
+        <v>64</v>
+      </c>
+      <c r="K41" t="s">
+        <v>64</v>
+      </c>
+      <c r="L41" t="s">
+        <v>64</v>
+      </c>
+      <c r="M41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="5">
+        <v>100</v>
+      </c>
+      <c r="E42" s="5">
+        <v>100</v>
+      </c>
+      <c r="F42" s="5">
+        <v>100</v>
+      </c>
+      <c r="G42" s="5">
+        <v>100</v>
+      </c>
+      <c r="H42" s="5">
+        <v>100</v>
+      </c>
+      <c r="I42" s="5"/>
+      <c r="M42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="6">
+        <v>100</v>
+      </c>
+      <c r="E43" s="6">
+        <v>100</v>
+      </c>
+      <c r="F43" s="6">
+        <v>100</v>
+      </c>
+      <c r="G43" s="6">
+        <v>100</v>
+      </c>
+      <c r="H43" s="6">
+        <v>100</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="M43">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="14">
+        <v>0</v>
+      </c>
+      <c r="E44" s="14">
+        <v>0</v>
+      </c>
+      <c r="F44" s="14">
+        <v>10</v>
+      </c>
+      <c r="G44" s="14">
+        <v>30</v>
+      </c>
+      <c r="H44" s="14">
+        <v>50</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J44" s="14">
+        <v>2025</v>
+      </c>
+      <c r="K44" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="L44" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="M44">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="14">
+        <v>0</v>
+      </c>
+      <c r="E45" s="14">
+        <v>0</v>
+      </c>
+      <c r="F45" s="14">
+        <v>0</v>
+      </c>
+      <c r="G45" s="14">
+        <v>10</v>
+      </c>
+      <c r="H45" s="14">
+        <v>30</v>
+      </c>
+      <c r="I45" s="14"/>
+      <c r="M45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="15">
+        <v>0</v>
+      </c>
+      <c r="E46" s="15">
+        <v>0</v>
+      </c>
+      <c r="F46" s="15">
+        <v>30</v>
+      </c>
+      <c r="G46" s="15">
+        <v>50</v>
+      </c>
+      <c r="H46" s="15">
+        <v>70</v>
+      </c>
+      <c r="I46" s="14"/>
+      <c r="M46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="12">
+        <v>0</v>
+      </c>
+      <c r="E47" s="12">
+        <v>0</v>
+      </c>
+      <c r="F47" s="12">
+        <v>1</v>
+      </c>
+      <c r="G47" s="12">
+        <v>3</v>
+      </c>
+      <c r="H47" s="12">
+        <v>5</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="J47" s="12">
+        <v>2028</v>
+      </c>
+      <c r="K47" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="L47" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="M47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D48" s="12">
+        <v>0</v>
+      </c>
+      <c r="E48" s="12">
+        <v>0</v>
+      </c>
+      <c r="F48" s="12">
+        <v>0</v>
+      </c>
+      <c r="G48" s="12">
+        <v>1</v>
+      </c>
+      <c r="H48" s="12">
+        <v>3</v>
+      </c>
+      <c r="I48" s="12"/>
+      <c r="M48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="13">
+        <v>0</v>
+      </c>
+      <c r="E49" s="13">
+        <v>0</v>
+      </c>
+      <c r="F49" s="13">
+        <v>3</v>
+      </c>
+      <c r="G49" s="13">
+        <v>5</v>
+      </c>
+      <c r="H49" s="13">
+        <v>9</v>
+      </c>
+      <c r="I49" s="12"/>
+      <c r="M49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="16">
+        <v>0</v>
+      </c>
+      <c r="E50" s="16">
+        <v>0</v>
+      </c>
+      <c r="F50" s="16">
+        <v>2</v>
+      </c>
+      <c r="G50" s="16">
+        <v>6</v>
+      </c>
+      <c r="H50" s="16">
+        <v>10</v>
+      </c>
+      <c r="I50" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="J50" s="16">
+        <v>2025</v>
+      </c>
+      <c r="K50" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="L50" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="M50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="16">
+        <v>0</v>
+      </c>
+      <c r="E51" s="16">
+        <v>0</v>
+      </c>
+      <c r="F51" s="16">
+        <v>0</v>
+      </c>
+      <c r="G51" s="16">
+        <v>2</v>
+      </c>
+      <c r="H51" s="16">
+        <v>5</v>
+      </c>
+      <c r="I51" s="16"/>
+      <c r="M51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="17">
+        <v>0</v>
+      </c>
+      <c r="E52" s="17">
+        <v>0</v>
+      </c>
+      <c r="F52" s="17">
+        <v>6</v>
+      </c>
+      <c r="G52" s="17">
+        <v>10</v>
+      </c>
+      <c r="H52" s="17">
+        <v>14</v>
+      </c>
+      <c r="I52" s="16"/>
+      <c r="M52">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEC8D20-7A52-476E-9A3F-F3ABE0AF0748}">
+  <dimension ref="A1:T18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="T1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="5">
+        <v>100</v>
+      </c>
+      <c r="H2" s="25">
+        <f>$Q$2</f>
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="24">
+        <f>$G$2</f>
+        <v>100</v>
+      </c>
+      <c r="J2" s="24">
+        <f t="shared" ref="J2:M2" si="0">$G$2</f>
+        <v>100</v>
+      </c>
+      <c r="K2" s="24">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="L2" s="24">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="M2" s="24">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="Q2" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="14">
+        <v>2020</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="G3" s="14">
+        <v>100</v>
+      </c>
+      <c r="H3" s="26">
+        <f t="shared" ref="H3:H18" si="1">$Q$2</f>
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="24">
+        <f>$G3*((1-EXP(-($E3+$F3)*MAX(I$1-$D3,0)))/(1+($F3/$E3)*EXP(-($E3+$F3)*MAX(I$1-$D3))))</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="24">
+        <f t="shared" ref="J3:M18" si="2">$G3*((1-EXP(-($E3+$F3)*MAX(J$1-$D3,0)))/(1+($F3/$E3)*EXP(-($E3+$F3)*MAX(J$1-$D3))))</f>
+        <v>42.679226553054164</v>
+      </c>
+      <c r="K3" s="24">
+        <f t="shared" si="2"/>
+        <v>91.858809388636558</v>
+      </c>
+      <c r="L3" s="24">
+        <f t="shared" si="2"/>
+        <v>99.955999987886514</v>
+      </c>
+      <c r="M3" s="24">
+        <f t="shared" si="2"/>
+        <v>99.999780279057944</v>
+      </c>
+      <c r="T3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="12">
+        <v>2020</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="12">
+        <v>100</v>
+      </c>
+      <c r="H4" s="27">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="24">
+        <f t="shared" ref="I4:I18" si="3">$G4*((1-EXP(-($E4+$F4)*MAX(I$1-$D4,0)))/(1+($F4/$E4)*EXP(-($E4+$F4)*MAX(I$1-$D4))))</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="24">
+        <f t="shared" si="2"/>
+        <v>15.411722829867564</v>
+      </c>
+      <c r="K4" s="24">
+        <f t="shared" si="2"/>
+        <v>42.181381367602278</v>
+      </c>
+      <c r="L4" s="24">
+        <f t="shared" si="2"/>
+        <v>87.971683418012475</v>
+      </c>
+      <c r="M4" s="24">
+        <f t="shared" si="2"/>
+        <v>98.523678563648915</v>
+      </c>
+      <c r="T4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="16">
+        <v>2015</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="G5" s="16">
+        <v>20</v>
+      </c>
+      <c r="H5" s="28">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="24">
+        <f t="shared" si="3"/>
+        <v>2.4101567986281616</v>
+      </c>
+      <c r="J5" s="24">
+        <f t="shared" si="2"/>
+        <v>5.5771257646543857</v>
+      </c>
+      <c r="K5" s="24">
+        <f t="shared" si="2"/>
+        <v>9.139925016931258</v>
+      </c>
+      <c r="L5" s="24">
+        <f t="shared" si="2"/>
+        <v>15.216367089632485</v>
+      </c>
+      <c r="M5" s="24">
+        <f t="shared" si="2"/>
+        <v>18.326040707377075</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="16">
+        <v>2020</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="G6" s="16">
+        <v>10</v>
+      </c>
+      <c r="H6" s="28">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="24">
+        <f t="shared" si="2"/>
+        <v>1.361478589715617</v>
+      </c>
+      <c r="K6" s="24">
+        <f t="shared" si="2"/>
+        <v>3.4484087661554712</v>
+      </c>
+      <c r="L6" s="24">
+        <f t="shared" si="2"/>
+        <v>7.7311613012867291</v>
+      </c>
+      <c r="M6" s="24">
+        <f t="shared" si="2"/>
+        <v>9.5044364808083692</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="5">
+        <v>100</v>
+      </c>
+      <c r="H7" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I7" s="24">
+        <f>$G$7</f>
+        <v>100</v>
+      </c>
+      <c r="J7" s="24">
+        <f t="shared" ref="J7:M7" si="4">$G$7</f>
+        <v>100</v>
+      </c>
+      <c r="K7" s="24">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="L7" s="24">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="M7" s="24">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="5">
+        <v>100</v>
+      </c>
+      <c r="H8" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="24">
+        <f>$G$8</f>
+        <v>100</v>
+      </c>
+      <c r="J8" s="24">
+        <f t="shared" ref="J8:M8" si="5">$G$8</f>
+        <v>100</v>
+      </c>
+      <c r="K8" s="24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="L8" s="24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="M8" s="24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2010</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>50</v>
+      </c>
+      <c r="H9" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="24">
+        <f t="shared" si="3"/>
+        <v>13.942814411635965</v>
+      </c>
+      <c r="J9" s="24">
+        <f t="shared" si="2"/>
+        <v>22.849812542328145</v>
+      </c>
+      <c r="K9" s="24">
+        <f t="shared" si="2"/>
+        <v>31.277120536322322</v>
+      </c>
+      <c r="L9" s="24">
+        <f t="shared" si="2"/>
+        <v>42.788155458708573</v>
+      </c>
+      <c r="M9" s="24">
+        <f t="shared" si="2"/>
+        <v>47.628653782953698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="12">
+        <v>2025</v>
+      </c>
+      <c r="E10" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="12">
+        <v>50</v>
+      </c>
+      <c r="H10" s="27">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="24">
+        <f t="shared" si="2"/>
+        <v>7.7058614149337821</v>
+      </c>
+      <c r="L10" s="24">
+        <f t="shared" si="2"/>
+        <v>35.180250825713841</v>
+      </c>
+      <c r="M10" s="24">
+        <f t="shared" si="2"/>
+        <v>47.840528378302047</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="12">
+        <v>2025</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="G11" s="12">
+        <v>60</v>
+      </c>
+      <c r="H11" s="27">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="24">
+        <f t="shared" si="2"/>
+        <v>8.1688715382937023</v>
+      </c>
+      <c r="L11" s="24">
+        <f t="shared" si="2"/>
+        <v>34.885635812064592</v>
+      </c>
+      <c r="M11" s="24">
+        <f t="shared" si="2"/>
+        <v>53.428293406629052</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="16">
+        <v>2028</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G12" s="16">
+        <v>100</v>
+      </c>
+      <c r="H12" s="28">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="24">
+        <f t="shared" si="2"/>
+        <v>7.8324976942203932</v>
+      </c>
+      <c r="L12" s="24">
+        <f t="shared" si="2"/>
+        <v>82.387974776626365</v>
+      </c>
+      <c r="M12" s="24">
+        <f t="shared" si="2"/>
+        <v>99.231981162990849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="16">
+        <v>2028</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.03</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="G13" s="16">
+        <v>100</v>
+      </c>
+      <c r="H13" s="28">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="24">
+        <f t="shared" si="2"/>
+        <v>7.8324976942203932</v>
+      </c>
+      <c r="L13" s="24">
+        <f t="shared" si="2"/>
+        <v>82.387974776626365</v>
+      </c>
+      <c r="M13" s="24">
+        <f t="shared" si="2"/>
+        <v>99.231981162990849</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="5">
+        <v>100</v>
+      </c>
+      <c r="H14" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="24">
+        <f>$G$14</f>
+        <v>100</v>
+      </c>
+      <c r="J14" s="24">
+        <f t="shared" ref="J14:L14" si="6">$G$14</f>
+        <v>100</v>
+      </c>
+      <c r="K14" s="24">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="L14" s="24">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="M14" s="24">
+        <f>$G$14</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="5">
+        <v>100</v>
+      </c>
+      <c r="H15" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="24">
+        <f>$G$15</f>
+        <v>100</v>
+      </c>
+      <c r="J15" s="24">
+        <f t="shared" ref="J15:M15" si="7">$G$15</f>
+        <v>100</v>
+      </c>
+      <c r="K15" s="24">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="L15" s="24">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="M15" s="24">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="14">
+        <v>2025</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="F16" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="G16" s="14">
+        <v>100</v>
+      </c>
+      <c r="H16" s="26">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="24">
+        <f t="shared" si="2"/>
+        <v>15.411722829867564</v>
+      </c>
+      <c r="L16" s="24">
+        <f t="shared" si="2"/>
+        <v>70.360501651427683</v>
+      </c>
+      <c r="M16" s="24">
+        <f t="shared" si="2"/>
+        <v>95.681056756604093</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2028</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="G17" s="12">
+        <v>20</v>
+      </c>
+      <c r="H17" s="27">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I17" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="24">
+        <f t="shared" si="2"/>
+        <v>0.82335631318545288</v>
+      </c>
+      <c r="L17" s="24">
+        <f t="shared" si="2"/>
+        <v>5.4662237455205522</v>
+      </c>
+      <c r="M17" s="24">
+        <f t="shared" si="2"/>
+        <v>10.229727402074349</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="16">
+        <v>2025</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="G18" s="16">
+        <v>15</v>
+      </c>
+      <c r="H18" s="28">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="24">
+        <f t="shared" si="2"/>
+        <v>2.0422178845734256</v>
+      </c>
+      <c r="L18" s="24">
+        <f t="shared" si="2"/>
+        <v>8.721408953016148</v>
+      </c>
+      <c r="M18" s="24">
+        <f t="shared" si="2"/>
+        <v>13.357073351657263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B18F167-6DBA-4198-BA06-95A49D6CEE47}">
   <dimension ref="A1:C19"/>
   <sheetViews>
@@ -3195,7 +5892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L460"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated bass diffusion implementation
Using yearly auxiliary variables
</commit_message>
<xml_diff>
--- a/Data/technological_maturity_readiness.xlsx
+++ b/Data/technological_maturity_readiness.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5C66B4-F855-4C0E-A3F8-491073ADB7B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB8F6C7-D552-4581-8C98-A745D1B27D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technological_readiness_bass" sheetId="6" r:id="rId1"/>
@@ -1091,7 +1091,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1179,7 @@
         <v>0.5</v>
       </c>
       <c r="I2" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J2" s="18">
         <f>$G$2</f>
@@ -1232,7 +1232,7 @@
         <v>0.5</v>
       </c>
       <c r="I3" s="10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J3" s="18">
         <f>$G3*((1-EXP(-($E3+$F3)*MAX(J$1-$D3,0)))/(1+($F3/$E3)*EXP(-($E3+$F3)*MAX(J$1-$D3))))</f>
@@ -1282,7 +1282,7 @@
         <v>0.5</v>
       </c>
       <c r="I4" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J4" s="18">
         <f t="shared" ref="J4:J18" si="3">$G4*((1-EXP(-($E4+$F4)*MAX(J$1-$D4,0)))/(1+($F4/$E4)*EXP(-($E4+$F4)*MAX(J$1-$D4))))</f>
@@ -1332,7 +1332,7 @@
         <v>0.5</v>
       </c>
       <c r="I5" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J5" s="18">
         <f t="shared" si="3"/>
@@ -1382,7 +1382,7 @@
         <v>0.5</v>
       </c>
       <c r="I6" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J6" s="18">
         <f t="shared" si="3"/>
@@ -1432,7 +1432,7 @@
         <v>0.5</v>
       </c>
       <c r="I7" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J7" s="18">
         <f>$G$7</f>
@@ -1482,7 +1482,7 @@
         <v>0.5</v>
       </c>
       <c r="I8" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J8" s="18">
         <f>$G$8</f>
@@ -1532,7 +1532,7 @@
         <v>0.5</v>
       </c>
       <c r="I9" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J9" s="18">
         <f t="shared" si="3"/>
@@ -1582,7 +1582,7 @@
         <v>0.5</v>
       </c>
       <c r="I10" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J10" s="18">
         <f t="shared" si="3"/>
@@ -1632,7 +1632,7 @@
         <v>0.5</v>
       </c>
       <c r="I11" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J11" s="18">
         <f t="shared" si="3"/>
@@ -1682,7 +1682,7 @@
         <v>0.5</v>
       </c>
       <c r="I12" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J12" s="18">
         <f t="shared" si="3"/>
@@ -1732,7 +1732,7 @@
         <v>0.5</v>
       </c>
       <c r="I13" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J13" s="18">
         <f t="shared" si="3"/>
@@ -1782,7 +1782,7 @@
         <v>0.5</v>
       </c>
       <c r="I14" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J14" s="18">
         <f>$G$14</f>
@@ -1832,7 +1832,7 @@
         <v>0.5</v>
       </c>
       <c r="I15" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J15" s="18">
         <f>$G$15</f>
@@ -1882,7 +1882,7 @@
         <v>0.5</v>
       </c>
       <c r="I16" s="10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J16" s="18">
         <f t="shared" si="3"/>
@@ -1932,7 +1932,7 @@
         <v>0.5</v>
       </c>
       <c r="I17" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J17" s="18">
         <f t="shared" si="3"/>
@@ -1982,7 +1982,7 @@
         <v>0.5</v>
       </c>
       <c r="I18" s="11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J18" s="18">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Emission Constraint + maturity update
Emission constraint
</commit_message>
<xml_diff>
--- a/Data/technological_maturity_readiness.xlsx
+++ b/Data/technological_maturity_readiness.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steffejb\OneDrive - NTNU\Work\GitHub\STraM_ntnu_development\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{820B5E57-E9EC-4642-A846-43C19011CF65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{E69D1286-6421-4EB1-9035-ECA5BACE0FFE}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="113_{7B03D4FF-8522-4FA3-AC78-48C68145C611}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{4247D5A8-7256-4CDE-BC62-3A6E3DBC8795}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technological_readiness_bass" sheetId="6" r:id="rId1"/>
@@ -1086,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EEC8D20-7A52-476E-9A3F-F3ABE0AF0748}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,13 +1219,13 @@
         <v>2020</v>
       </c>
       <c r="E3" s="5">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="F3" s="5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G3" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H3" s="14">
         <f t="shared" si="0"/>
@@ -1236,23 +1236,23 @@
       </c>
       <c r="J3" s="12">
         <f>$G3*((1-EXP(-($E3+$F3)*MAX(J$1-$D3,0)))/(1+($F3/$E3)*EXP(-($E3+$F3)*MAX(J$1-$D3))))</f>
-        <v>9.6474574562864284</v>
+        <v>4.718929306551364</v>
       </c>
       <c r="K3" s="12">
         <f t="shared" ref="K3:N13" si="2">$G3*((1-EXP(-($E3+$F3)*MAX(K$1-$D3,0)))/(1+($F3/$E3)*EXP(-($E3+$F3)*MAX(K$1-$D3))))</f>
-        <v>56.607264701041494</v>
+        <v>28.193872913196202</v>
       </c>
       <c r="L3" s="12">
         <f t="shared" si="2"/>
-        <v>91.858809388636558</v>
+        <v>60.619781921478939</v>
       </c>
       <c r="M3" s="12">
         <f t="shared" si="2"/>
-        <v>99.955999987886514</v>
+        <v>79.623914283155713</v>
       </c>
       <c r="N3" s="12">
         <f t="shared" si="2"/>
-        <v>99.999780279057944</v>
+        <v>79.994335396429236</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -1266,16 +1266,16 @@
         <v>22</v>
       </c>
       <c r="D4" s="6">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="E4" s="6">
         <v>0.02</v>
       </c>
       <c r="F4" s="6">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G4" s="6">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H4" s="15">
         <f t="shared" si="0"/>
@@ -1286,23 +1286,23 @@
       </c>
       <c r="J4" s="12">
         <f t="shared" ref="J4:J13" si="3">$G4*((1-EXP(-($E4+$F4)*MAX(J$1-$D4,0)))/(1+($F4/$E4)*EXP(-($E4+$F4)*MAX(J$1-$D4))))</f>
-        <v>4.7842225034986816</v>
+        <v>2.0724939854319051</v>
       </c>
       <c r="K4" s="12">
         <f t="shared" si="2"/>
-        <v>19.961706055232963</v>
+        <v>17.830518721584536</v>
       </c>
       <c r="L4" s="12">
         <f t="shared" si="2"/>
-        <v>42.181381367602278</v>
+        <v>46.116657159583688</v>
       </c>
       <c r="M4" s="12">
         <f t="shared" si="2"/>
-        <v>87.971683418012475</v>
+        <v>86.814365052467252</v>
       </c>
       <c r="N4" s="12">
         <f t="shared" si="2"/>
-        <v>98.523678563648915</v>
+        <v>89.865877228933556</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1416,16 +1416,16 @@
         <v>22</v>
       </c>
       <c r="D7" s="3">
-        <v>2010</v>
+        <v>2025</v>
       </c>
       <c r="E7" s="3">
         <v>0.02</v>
       </c>
       <c r="F7" s="3">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="G7" s="3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H7" s="13">
         <f t="shared" si="0"/>
@@ -1436,23 +1436,23 @@
       </c>
       <c r="J7" s="12">
         <f t="shared" si="3"/>
-        <v>17.464494442273157</v>
+        <v>0</v>
       </c>
       <c r="K7" s="12">
         <f t="shared" si="2"/>
-        <v>24.621347263899171</v>
+        <v>1.3466991251383984</v>
       </c>
       <c r="L7" s="12">
         <f t="shared" si="2"/>
-        <v>31.277120536322322</v>
+        <v>10.481205096735865</v>
       </c>
       <c r="M7" s="12">
         <f t="shared" si="2"/>
-        <v>42.788155458708573</v>
+        <v>48.411595582463747</v>
       </c>
       <c r="N7" s="12">
         <f t="shared" si="2"/>
-        <v>47.628653782953698</v>
+        <v>59.06526823681439</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1466,16 +1466,16 @@
         <v>22</v>
       </c>
       <c r="D8" s="6">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="E8" s="6">
         <v>0.02</v>
       </c>
       <c r="F8" s="6">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G8" s="6">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="H8" s="15">
         <f t="shared" si="0"/>
@@ -1490,19 +1490,19 @@
       </c>
       <c r="K8" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.0724939854319051</v>
       </c>
       <c r="L8" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17.830518721584536</v>
       </c>
       <c r="M8" s="12">
         <f t="shared" si="2"/>
-        <v>21.090690683801139</v>
+        <v>79.451354510710701</v>
       </c>
       <c r="N8" s="12">
         <f t="shared" si="2"/>
-        <v>43.985841709006237</v>
+        <v>89.519352405398095</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1516,16 +1516,16 @@
         <v>22</v>
       </c>
       <c r="D9" s="6">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="E9" s="6">
         <v>0.02</v>
       </c>
       <c r="F9" s="6">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="G9" s="6">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H9" s="15">
         <f t="shared" si="0"/>
@@ -1540,19 +1540,19 @@
       </c>
       <c r="K9" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.8422168759394713</v>
       </c>
       <c r="L9" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15.849349974741809</v>
       </c>
       <c r="M9" s="12">
         <f t="shared" si="2"/>
-        <v>20.690452596932829</v>
+        <v>70.623426231742854</v>
       </c>
       <c r="N9" s="12">
         <f t="shared" si="2"/>
-        <v>46.386967807720374</v>
+        <v>79.572757693687194</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1666,16 +1666,16 @@
         <v>22</v>
       </c>
       <c r="D12" s="5">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="E12" s="5">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F12" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G12" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H12" s="14">
         <f t="shared" si="0"/>
@@ -1690,19 +1690,19 @@
       </c>
       <c r="K12" s="12">
         <f t="shared" si="2"/>
-        <v>2.1881117876254099</v>
+        <v>19.38708935850411</v>
       </c>
       <c r="L12" s="12">
         <f t="shared" si="2"/>
-        <v>15.411722829867564</v>
+        <v>54.243954206266721</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" si="2"/>
-        <v>70.360501651427683</v>
+        <v>79.503995228273482</v>
       </c>
       <c r="N12" s="12">
         <f t="shared" si="2"/>
-        <v>95.681056756604093</v>
+        <v>79.993231421914444</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1716,16 +1716,16 @@
         <v>22</v>
       </c>
       <c r="D13" s="6">
-        <v>2028</v>
+        <v>2024</v>
       </c>
       <c r="E13" s="6">
         <v>0.02</v>
       </c>
       <c r="F13" s="6">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="G13" s="6">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="H13" s="15">
         <f t="shared" si="0"/>
@@ -1740,19 +1740,19 @@
       </c>
       <c r="K13" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.3087954698702839</v>
       </c>
       <c r="L13" s="12">
         <f t="shared" si="2"/>
-        <v>0.82335631318545288</v>
+        <v>31.718107027345727</v>
       </c>
       <c r="M13" s="12">
         <f t="shared" si="2"/>
-        <v>5.4662237455205522</v>
+        <v>87.773372987202734</v>
       </c>
       <c r="N13" s="12">
         <f t="shared" si="2"/>
-        <v>10.229727402074349</v>
+        <v>89.965817097308673</v>
       </c>
     </row>
   </sheetData>
@@ -1765,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76863746-C34D-4AED-8106-1FF68650C184}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>